<commit_message>
Casos canje de credito
</commit_message>
<xml_diff>
--- a/LineasClubPersonalBack.xlsx
+++ b/LineasClubPersonalBack.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A674155\eclipse-workspace\WebPersonal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6AC8614C-EDF4-4C17-B0B5-E9B81DA9C1E1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{702E7E90-B959-4682-9106-7C78C86F078A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Linea</t>
   </si>
@@ -67,6 +67,27 @@
   </si>
   <si>
     <t>Busqueda_por_Documento_PRE</t>
+  </si>
+  <si>
+    <t>Canje_de_Puntos_Canje_de_Voucher_MIX</t>
+  </si>
+  <si>
+    <t>Canje_de_Puntos_Canje_de_Voucher_POS</t>
+  </si>
+  <si>
+    <t>Canje_de_Puntos_Canje_de_Voucher_PRE</t>
+  </si>
+  <si>
+    <t>Canje_de_Puntos_Canje_de_Credito_MIX</t>
+  </si>
+  <si>
+    <t>Canje_de_Puntos_Canje_de_Credito_PRE</t>
+  </si>
+  <si>
+    <t>Resumen_de_Puntos_MIX</t>
+  </si>
+  <si>
+    <t>Resumen_de_Puntos_POS</t>
   </si>
 </sst>
 </file>
@@ -129,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -137,7 +158,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -424,7 +444,7 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,7 +465,7 @@
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <v>1162816939</v>
       </c>
       <c r="C2" s="3"/>
@@ -463,7 +483,7 @@
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>1145642605</v>
       </c>
     </row>
@@ -471,7 +491,7 @@
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>1162676705</v>
       </c>
     </row>
@@ -479,7 +499,7 @@
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>1162816939</v>
       </c>
     </row>
@@ -487,7 +507,7 @@
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>1145642605</v>
       </c>
     </row>
@@ -495,7 +515,7 @@
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>1162676705</v>
       </c>
     </row>
@@ -503,7 +523,7 @@
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>1162816939</v>
       </c>
     </row>
@@ -511,7 +531,7 @@
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>1145642605</v>
       </c>
     </row>
@@ -519,7 +539,7 @@
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>1162676705</v>
       </c>
     </row>
@@ -527,7 +547,7 @@
       <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <v>1162816939</v>
       </c>
     </row>
@@ -535,7 +555,7 @@
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="5">
         <v>1145642605</v>
       </c>
     </row>
@@ -543,32 +563,81 @@
       <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <v>1162676705</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="4"/>
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="5">
+        <v>1162816939</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="5"/>
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="5">
+        <v>1145642605</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="5"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="4"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="4"/>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="5">
+        <v>1162676705</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="5">
+        <v>1162816939</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="5">
+        <v>1162676705</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="5">
+        <v>1162816939</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="5">
+        <v>1145642605</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="5">
+        <v>1162676705</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B24" s="4"/>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Caso actualizacion datos club back
</commit_message>
<xml_diff>
--- a/LineasClubPersonalBack.xlsx
+++ b/LineasClubPersonalBack.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A674155\eclipse-workspace\WebPersonal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{938D68B4-EFCA-46AA-8629-4E48E89A3F90}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5AD90414-3CD1-4A29-995D-19CF829D1C37}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Linea</t>
   </si>
@@ -97,6 +97,15 @@
   </si>
   <si>
     <t>Resumen_de_Puntos_PRE</t>
+  </si>
+  <si>
+    <t>Actualizacion_de_Datos_MIX</t>
+  </si>
+  <si>
+    <t>Actualizacion_de_Datos_POS</t>
+  </si>
+  <si>
+    <t>Actualizacion_de_Datos_PRE</t>
   </si>
 </sst>
 </file>
@@ -452,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,7 +666,28 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="4"/>
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="5">
+        <v>1162816939</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="5">
+        <v>1145642605</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="5">
+        <v>1162676705</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>

</xml_diff>

<commit_message>
Lineas para caso Movimientos_de_Puntos_MIX
LIneas para caso Movimientos_de_Puntos_MIX
</commit_message>
<xml_diff>
--- a/LineasClubPersonalBack.xlsx
+++ b/LineasClubPersonalBack.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A674155\eclipse-workspace\WebPersonal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Telecom\WebPersonal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{938D68B4-EFCA-46AA-8629-4E48E89A3F90}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F8EE6465-A490-4667-87AB-4BDFE34BC644}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Linea</t>
   </si>
@@ -97,6 +97,15 @@
   </si>
   <si>
     <t>Resumen_de_Puntos_PRE</t>
+  </si>
+  <si>
+    <t>Movimientos_de_Puntos_MIX</t>
+  </si>
+  <si>
+    <t>Movimientos_de_Puntos_POS</t>
+  </si>
+  <si>
+    <t>Movimientos_de_Puntos_PRE</t>
   </si>
 </sst>
 </file>
@@ -452,11 +461,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
@@ -657,7 +666,28 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="4"/>
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="5">
+        <v>1162816939</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="5">
+        <v>1145642605</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="5">
+        <v>1162676705</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>

</xml_diff>

<commit_message>
Lineas para Canjes realizados
Lineas para Canjes realizados
</commit_message>
<xml_diff>
--- a/LineasClubPersonalBack.xlsx
+++ b/LineasClubPersonalBack.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Telecom\WebPersonal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F8EE6465-A490-4667-87AB-4BDFE34BC644}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{65742F03-234B-48DD-89FE-0EBDF29DF1AB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Linea</t>
   </si>
@@ -106,6 +106,15 @@
   </si>
   <si>
     <t>Movimientos_de_Puntos_PRE</t>
+  </si>
+  <si>
+    <t>Canjes_Realizados_MIX</t>
+  </si>
+  <si>
+    <t>Canjes_Realizados_POS</t>
+  </si>
+  <si>
+    <t>Canjes_Realizados_PRE</t>
   </si>
 </sst>
 </file>
@@ -168,14 +177,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -459,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,7 +489,7 @@
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>1162816939</v>
       </c>
       <c r="C2" s="3"/>
@@ -501,7 +507,7 @@
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>1145642605</v>
       </c>
     </row>
@@ -509,7 +515,7 @@
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>1162676705</v>
       </c>
     </row>
@@ -517,7 +523,7 @@
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>1162816939</v>
       </c>
     </row>
@@ -525,7 +531,7 @@
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>1145642605</v>
       </c>
     </row>
@@ -533,7 +539,7 @@
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>1162676705</v>
       </c>
     </row>
@@ -541,7 +547,7 @@
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>1162816939</v>
       </c>
     </row>
@@ -549,7 +555,7 @@
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>1145642605</v>
       </c>
     </row>
@@ -557,7 +563,7 @@
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>1162676705</v>
       </c>
     </row>
@@ -565,7 +571,7 @@
       <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="4">
         <v>1162816939</v>
       </c>
     </row>
@@ -573,7 +579,7 @@
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="4">
         <v>1145642605</v>
       </c>
     </row>
@@ -581,7 +587,7 @@
       <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="4">
         <v>1162676705</v>
       </c>
     </row>
@@ -589,7 +595,7 @@
       <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="4">
         <v>1162816939</v>
       </c>
     </row>
@@ -597,7 +603,7 @@
       <c r="A15" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="4">
         <v>1145642605</v>
       </c>
     </row>
@@ -605,7 +611,7 @@
       <c r="A16" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="4">
         <v>1162676705</v>
       </c>
     </row>
@@ -613,7 +619,7 @@
       <c r="A17" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="4">
         <v>1162816939</v>
       </c>
     </row>
@@ -621,7 +627,7 @@
       <c r="A18" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="4">
         <v>1162676705</v>
       </c>
     </row>
@@ -629,7 +635,7 @@
       <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="4">
         <v>1162816939</v>
       </c>
     </row>
@@ -637,7 +643,7 @@
       <c r="A20" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="4">
         <v>1145642605</v>
       </c>
     </row>
@@ -645,7 +651,7 @@
       <c r="A21" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="4">
         <v>1162676705</v>
       </c>
     </row>
@@ -653,7 +659,7 @@
       <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="4">
         <v>1162816939</v>
       </c>
     </row>
@@ -661,7 +667,7 @@
       <c r="A23" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="4">
         <v>1162676705</v>
       </c>
     </row>
@@ -669,7 +675,7 @@
       <c r="A24" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="4">
         <v>1162816939</v>
       </c>
     </row>
@@ -677,7 +683,7 @@
       <c r="A25" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="4">
         <v>1145642605</v>
       </c>
     </row>
@@ -685,12 +691,33 @@
       <c r="A26" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="4">
         <v>1162676705</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="4"/>
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="4">
+        <v>1162816939</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="4">
+        <v>1145642605</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="4">
+        <v>1162676705</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Actualizacion excel club back
</commit_message>
<xml_diff>
--- a/LineasClubPersonalBack.xlsx
+++ b/LineasClubPersonalBack.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Telecom\WebPersonal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A674155\eclipse-workspace\WebPersonal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{65742F03-234B-48DD-89FE-0EBDF29DF1AB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E0596B29-A4C0-4F9F-A6DB-4AA71213D3E1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Linea</t>
   </si>
@@ -115,6 +115,24 @@
   </si>
   <si>
     <t>Canjes_Realizados_PRE</t>
+  </si>
+  <si>
+    <t>ABM_Usuarios_MIX</t>
+  </si>
+  <si>
+    <t>ABM_Usuarios_POS</t>
+  </si>
+  <si>
+    <t>ABM_Usuarios_PRE</t>
+  </si>
+  <si>
+    <t>Actualizacion_de_Datos_MIX</t>
+  </si>
+  <si>
+    <t>Actualizacion_de_Datos_POS</t>
+  </si>
+  <si>
+    <t>Actualizacion_de_Datos_PRE</t>
   </si>
 </sst>
 </file>
@@ -465,13 +483,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
@@ -719,6 +737,54 @@
         <v>1162676705</v>
       </c>
     </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="4">
+        <v>1162816939</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="4">
+        <v>1145642605</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="4">
+        <v>1162676705</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="4">
+        <v>1162816939</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="4">
+        <v>1145642605</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="4">
+        <v>1162676705</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Se actualiza excel con lineas club back
</commit_message>
<xml_diff>
--- a/LineasClubPersonalBack.xlsx
+++ b/LineasClubPersonalBack.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A674155\eclipse-workspace\WebPersonal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CD1108FE-E432-4F00-803C-5CA59B0191FD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D7572E1F-2786-452F-96C6-23233A6AAF3D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Linea</t>
   </si>
@@ -142,13 +142,22 @@
   </si>
   <si>
     <t>Anulacion_Canje_de_premio_Diferido_PRE</t>
+  </si>
+  <si>
+    <t>Adhesion_Linea_Usuario_MIX</t>
+  </si>
+  <si>
+    <t>Adhesion_Linea_Usuario_POS</t>
+  </si>
+  <si>
+    <t>Adhesion_Linea_Usuario_PRE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,6 +186,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -204,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -212,6 +227,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L38"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,6 +834,30 @@
         <v>1162676705</v>
       </c>
     </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="4">
+        <v>1162786772</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="4">
+        <v>1156393564</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="4">
+        <v>1162678774</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualizacion orden de ejecucion casos club back
</commit_message>
<xml_diff>
--- a/LineasClubPersonalBack.xlsx
+++ b/LineasClubPersonalBack.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A674155\eclipse-workspace\WebPersonal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D7572E1F-2786-452F-96C6-23233A6AAF3D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{697AC267-DAB1-49D2-A55E-4AEA1257E1F3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -157,7 +157,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,12 +186,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -219,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -227,7 +221,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -510,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,7 +828,7 @@
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
+      <c r="A39" t="s">
         <v>39</v>
       </c>
       <c r="B39" s="4">
@@ -843,7 +836,7 @@
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
+      <c r="A40" t="s">
         <v>40</v>
       </c>
       <c r="B40" s="4">
@@ -851,7 +844,7 @@
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
+      <c r="A41" t="s">
         <v>41</v>
       </c>
       <c r="B41" s="4">

</xml_diff>